<commit_message>
fix. skill card table
</commit_message>
<xml_diff>
--- a/101_table_skill_card.xlsx
+++ b/101_table_skill_card.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr codeName="현재_통합_문서"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AjouMSE\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\과제폴더\MSE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D60F9E4-3585-48AF-A46E-E4DB009B8D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF281E3-C892-4BA5-8BCB-E747602F0C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="686" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="686" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="10" r:id="rId1"/>
     <sheet name="data" sheetId="2" r:id="rId2"/>
+    <sheet name="range" sheetId="11" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">data!$A$3:$K$3</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="142">
   <si>
     <t>설명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -127,15 +130,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>오른쪽</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Right</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>왼쪽</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -143,15 +138,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>위쪽</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Up</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아래쪽</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -175,10 +162,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>//0: 이동, 100: 공격</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Wind Cutter</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -187,21 +170,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>윈드커터</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>파이어볼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>//인게임 텍스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스킬 구분
-0: 이동
-100: 공격</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -213,13 +182,432 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>우선순위
-1~999
-낮을수록 먼저 발동</t>
+    <t>Explosion</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>값</t>
+    <t>Magic Arrow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Combustion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lightning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ice Spear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Earth Break</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Meteor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cyclone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Life Recovery</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mana Overload</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Concentration</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mana Charge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cleanse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mana Disorder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Torrential Tribute</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fire Storm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Water Bomb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flamethrower</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Double Right</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Double Left</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Double Up</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Double Down</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mana Shield</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>익스플로전</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동(우)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동(좌)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동(상)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동(하)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화염구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마법 화살</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>발화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>라이트닝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이스 스피어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메테오</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>싸이클론</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>라이프 리커버리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마나 실드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마나 오버로드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마나 차지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정신집중</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마나 디스오더</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>격류장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화염폭풍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>칼날바람</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Super Nova</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>슈퍼노바</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>워터 밤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대지 파괴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화염방사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화염강타</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flame Smash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이중 이동(우)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이중 이동(좌)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이중 이동(상)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이중 이동(하)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>102100003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>102100004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>102100005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>102100006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>102100007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>102100008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>102100009</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>102100010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>201100001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>102100011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>102100012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>102100013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>102100014</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>102100015</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>102100016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>102000005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>102000006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>102000007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>102000008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우선순위
+0~2
+낮을수록 먼저 발동
+이동 : 0
+특수행동 : 1
+공격 : 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>값(Ex. Skill Damage….)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>십자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3*3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5*5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>checkrange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>effectrange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1*1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//1 이동, 100: 공격</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스킬 구분
+1: 이동
+100: 공격
+200: 특수행동</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -317,7 +705,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -345,6 +733,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -552,7 +946,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -641,6 +1035,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1042,7 +1442,7 @@
   <dimension ref="A1:C16298"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1121,7 +1521,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="33.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>18</v>
       </c>
@@ -1129,7 +1529,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>41</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1140,7 +1540,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1151,10 +1551,10 @@
         <v>16</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="33.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="67.5" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>21</v>
       </c>
@@ -1162,7 +1562,7 @@
         <v>16</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>44</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1173,7 +1573,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>45</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -50044,13 +50444,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" sqref="A1:K3"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -50151,22 +50551,22 @@
         <v>8</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I3" s="24" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -50184,10 +50584,10 @@
         <v>0</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4" s="29">
         <v>1</v>
@@ -50199,7 +50599,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="29">
-        <v>9999</v>
+        <v>0</v>
       </c>
       <c r="K4" s="25">
         <v>0</v>
@@ -50220,10 +50620,10 @@
         <v>1</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G5" s="29">
         <v>1</v>
@@ -50235,7 +50635,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="29">
-        <v>9999</v>
+        <v>0</v>
       </c>
       <c r="K5" s="25">
         <v>0</v>
@@ -50256,10 +50656,10 @@
         <v>2</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G6" s="29">
         <v>1</v>
@@ -50271,7 +50671,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="29">
-        <v>9999</v>
+        <v>0</v>
       </c>
       <c r="K6" s="25">
         <v>0</v>
@@ -50292,10 +50692,10 @@
         <v>3</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G7" s="29">
         <v>1</v>
@@ -50307,7 +50707,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="29">
-        <v>9999</v>
+        <v>0</v>
       </c>
       <c r="K7" s="25">
         <v>0</v>
@@ -50328,10 +50728,10 @@
         <v>0</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G8" s="2">
         <v>100</v>
@@ -50343,7 +50743,7 @@
         <v>1</v>
       </c>
       <c r="J8" s="2">
-        <v>9999</v>
+        <v>2</v>
       </c>
       <c r="K8" s="25">
         <v>10</v>
@@ -50364,10 +50764,10 @@
         <v>1</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G9" s="2">
         <v>100</v>
@@ -50379,10 +50779,885 @@
         <v>3</v>
       </c>
       <c r="J9" s="2">
-        <v>9999</v>
+        <v>2</v>
       </c>
       <c r="K9" s="25">
         <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>101100002</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="2">
+        <v>100</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="J10" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="K10" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>101100003</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="2">
+        <v>100</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="I11" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="J11" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="K11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>101100004</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="2">
+        <v>100</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="I12" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="J12" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="K12" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>101100005</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="2">
+        <v>100</v>
+      </c>
+      <c r="H13" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="I13" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="J13" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="K13" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>101100006</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="2">
+        <v>100</v>
+      </c>
+      <c r="H14" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="I14" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="J14" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="K14" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>101100007</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="2">
+        <v>100</v>
+      </c>
+      <c r="H15" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="I15" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="J15" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="K15" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>101100008</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="2">
+        <v>100</v>
+      </c>
+      <c r="H16" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="I16" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="J16" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="K16" s="2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>101100009</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="2">
+        <v>100</v>
+      </c>
+      <c r="H17" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="I17" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="J17" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="K17" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>101200000</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="2">
+        <v>200</v>
+      </c>
+      <c r="H18" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="I18" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="J18" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="K18" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>101200001</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" s="2">
+        <v>200</v>
+      </c>
+      <c r="H19" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="I19" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="J19" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="K19" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>101200002</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="2">
+        <v>200</v>
+      </c>
+      <c r="H20" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="I20" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="J20" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>101200003</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" s="2">
+        <v>200</v>
+      </c>
+      <c r="H21" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="I21" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="J21" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="K21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>101200004</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" s="2">
+        <v>200</v>
+      </c>
+      <c r="H22" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="I22" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="J22" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="K22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>101200005</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" s="2">
+        <v>200</v>
+      </c>
+      <c r="H23" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="I23" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="J23" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="K23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>101200006</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G24" s="2">
+        <v>200</v>
+      </c>
+      <c r="H24" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="I24" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="J24" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="K24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>101200007</v>
+      </c>
+      <c r="B25" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G25" s="2">
+        <v>100</v>
+      </c>
+      <c r="H25" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="I25" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="J25" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="K25" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>101100010</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G26" s="2">
+        <v>100</v>
+      </c>
+      <c r="H26" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="I26" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="J26" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="K26" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>101100011</v>
+      </c>
+      <c r="B27" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G27" s="2">
+        <v>100</v>
+      </c>
+      <c r="H27" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="I27" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="J27" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="K27" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>101100012</v>
+      </c>
+      <c r="B28" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" s="2">
+        <v>100</v>
+      </c>
+      <c r="H28" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="I28" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="J28" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="K28" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>101100013</v>
+      </c>
+      <c r="B29" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G29" s="2">
+        <v>100</v>
+      </c>
+      <c r="H29" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="I29" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="J29" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="K29" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>101100014</v>
+      </c>
+      <c r="B30" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G30" s="2">
+        <v>100</v>
+      </c>
+      <c r="H30" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="I30" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="J30" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="K30" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>101000004</v>
+      </c>
+      <c r="B31" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31" s="2">
+        <v>1</v>
+      </c>
+      <c r="H31" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="I31" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="J31" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="K31" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>101000005</v>
+      </c>
+      <c r="B32" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G32" s="2">
+        <v>1</v>
+      </c>
+      <c r="H32" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="I32" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="J32" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="K32" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>101000006</v>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G33" s="2">
+        <v>1</v>
+      </c>
+      <c r="H33" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="I33" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="J33" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="K33" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>101000007</v>
+      </c>
+      <c r="B34" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G34" s="2">
+        <v>1</v>
+      </c>
+      <c r="H34" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="I34" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="J34" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="K34" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -50390,7 +51665,7 @@
   <conditionalFormatting sqref="A10:A1048576">
     <cfRule type="duplicateValues" dxfId="14" priority="220"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H10:H1048576 J10:J1048576">
+  <conditionalFormatting sqref="J10:J1048576 H10:H1048576">
     <cfRule type="colorScale" priority="133">
       <colorScale>
         <cfvo type="min"/>
@@ -50461,7 +51736,97 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B10:D10 B11:D1048576" numberStoredAsText="1"/>
+    <ignoredError sqref="B36:D1048576 C35:D35" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85130162-33F8-409D-8E0D-12A607C65466}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="55.875" customWidth="1"/>
+    <col min="6" max="6" width="36.875" customWidth="1"/>
+    <col min="7" max="7" width="11.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>134</v>
+      </c>
+      <c r="H4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>135</v>
+      </c>
+      <c r="H5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>136</v>
+      </c>
+      <c r="H6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>